<commit_message>
feat: add environment configuration and enhance novelty model
- Add .env files support with example configuration
- Update .gitignore to include environment files
- Extend NoveltyModel with additional fields
- Add environment-based scripts in package.json
- Update README with installation and configuration instructions
- Modify API endpoints and auth flow to use environment variables
- Enhance index.ts with complete novelty payload and environment variables
</commit_message>
<xml_diff>
--- a/assets/prod.xlsx
+++ b/assets/prod.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/korbold/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/korbold/Documents/Kruger/Favorita/Script Filiales/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288FE19C-253C-584F-8B22-8253C0827E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C4ACB3-6579-3C47-8D35-04F2DFCB03B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="27240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="INFRACCIÓN">#REF!</definedName>
     <definedName name="PROVEEDOR">Listas!C2:C5</definedName>
     <definedName name="Selección">Formulario!#REF!</definedName>
-    <definedName name="Seleción">Formulario!$A$4:$A$1048576</definedName>
+    <definedName name="Seleción">Formulario!$A$2:$A$1048576</definedName>
     <definedName name="TIPO_DOCUMENTO">Listas!D2:D4</definedName>
     <definedName name="TRABAJADOR">Listas!$B$2:$B$5</definedName>
     <definedName name="TRABAJADORES">Listas!$B$2:$B$5</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -63,9 +63,6 @@
     <t>SEGUNDO APELLIDO</t>
   </si>
   <si>
-    <t>CEDULA</t>
-  </si>
-  <si>
     <t>PASAPORTE</t>
   </si>
   <si>
@@ -105,18 +102,9 @@
     <t>CATEGORIAS</t>
   </si>
   <si>
-    <t>máximo 10 caracteres</t>
-  </si>
-  <si>
-    <t>máximo 25 caracteres</t>
-  </si>
-  <si>
     <t>FECHA NOVEDAD</t>
   </si>
   <si>
-    <t>máximo 100 caracteres</t>
-  </si>
-  <si>
     <t>COLOR</t>
   </si>
   <si>
@@ -145,9 +133,6 @@
   </si>
   <si>
     <t>RAZON SOCIAL DE FILIAL</t>
-  </si>
-  <si>
-    <t>LAS CELDAS DE COLOR SON CAMPOS OBLIGATORIOS</t>
   </si>
   <si>
     <t>0920172483</t>
@@ -279,20 +264,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -525,173 +502,151 @@
   <sheetPr codeName="Hoja1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="19.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.1640625" style="5" customWidth="1"/>
-    <col min="17" max="16384" width="12.6640625" style="5"/>
+    <col min="1" max="1" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="19.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.1640625" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="12.6640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="7">
+        <v>28964</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="12">
+        <v>1790746119001</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="11">
-        <v>28964</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="16">
-        <v>1790746119001</v>
-      </c>
-      <c r="P4" s="15" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"CLIENTE,TRABAJOR,PROVEEDOR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>TIPO_DOCUMENTO</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>INDIRECT(A3)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B2" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>INDIRECT(A1)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -703,13 +658,13 @@
           <x14:formula1>
             <xm:f>Listas!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>A4</xm:sqref>
+          <xm:sqref>A2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>Listas!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>N4</xm:sqref>
+          <xm:sqref>N2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -736,69 +691,69 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add Windows support and improve file path handling
- Update Excel file path handling to use path.join for cross-platform compatibility
- Add Windows-specific npm scripts for environment setup
- Include dotenv as explicit dependency
- Update README with Windows instructions and cross-platform notes
</commit_message>
<xml_diff>
--- a/assets/prod.xlsx
+++ b/assets/prod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/korbold/Documents/Kruger/Favorita/Script Filiales/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C4ACB3-6579-3C47-8D35-04F2DFCB03B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4135D62-4B13-ED40-9C87-445058969960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="27240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>19/06/2025</t>
-  </si>
-  <si>
-    <t>08:14:14 AM</t>
   </si>
   <si>
     <t>Cuenta en Legal</t>
@@ -505,7 +502,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -618,14 +615,12 @@
       <c r="J2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>24</v>

</xml_diff>